<commit_message>
[svn r40] Handle missing rows in XLSX files. Handle #d/#u z-level transformations properly, including with multilayer blueprints. Improved robustness of file importer, esp. getting the layer sizing correct. Refactored blueprint level functionality to blueprint.py. Refactored qfconvert.py to support profiling as a command line option (not yet done). Transformer de-classed; just using the bare functions at package level instead. Added util.Struct class to simplify creating classes that follow a "struct+functions" pattern. Added Alt+E replay support to AHK. Polished transformation dialog/s. Handle qfconvert-outputted exceptions within AHK (show to user via MsgBox). More exceptions. Cleanup. Updated tests. Changed sublime project build type to Python.
--HG--
branch : trunk
</commit_message>
<xml_diff>
--- a/blueprints/Tests/transform-test.xlsx
+++ b/blueprints/Tests/transform-test.xlsx
@@ -16,15 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="3">
   <si>
     <t>d</t>
   </si>
   <si>
-    <t>#dig Transform test. Try this with a transform of 'fliph 2e flipv 2s 10e 10s'</t>
+    <t>#</t>
   </si>
   <si>
-    <t>#</t>
+    <t xml:space="preserve">#dig Transform test. </t>
   </si>
 </sst>
 </file>
@@ -356,84 +356,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="17.25" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" customHeight="1">
+    <row r="1" spans="1:10" ht="17.25" customHeight="1">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17.25" customHeight="1">
-      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1">
-      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17.25" customHeight="1">
-      <c r="H5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1">
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1">
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
-        <v>0</v>
-      </c>
       <c r="I7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1">
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="s">
@@ -445,20 +472,17 @@
       <c r="F8" t="s">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
-        <v>0</v>
-      </c>
       <c r="I8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17.25" customHeight="1">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17.25" customHeight="1">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
@@ -474,40 +498,75 @@
       <c r="G9" t="s">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
-        <v>0</v>
-      </c>
       <c r="I9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17.25" customHeight="1">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>